<commit_message>
added completed password manager
</commit_message>
<xml_diff>
--- a/password_manager/data/password.xlsx
+++ b/password_manager/data/password.xlsx
@@ -439,39 +439,39 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>tiktok</t>
+          <t>vk</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>vk</t>
+          <t>mail</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>qwerty12</t>
+          <t>qwer12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>telega10</t>
+          <t>asdc1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>mail09</t>
+          <t>tyhe56</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>videohahah</t>
+          <t>hello97</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>zxcv774</t>
+          <t>pochta</t>
         </is>
       </c>
     </row>

</xml_diff>